<commit_message>
padam edited and finalized nabin sir, sundar basti file
</commit_message>
<xml_diff>
--- a/ofc/estimates/estimate for pahiro/पासिखेल पहिरो बाटो संचालन.xlsx
+++ b/ofc/estimates/estimate for pahiro/पासिखेल पहिरो बाटो संचालन.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="new" sheetId="18" r:id="rId1"/>
@@ -614,26 +614,10 @@
     <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -644,6 +628,37 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -665,21 +680,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1432,113 +1432,113 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="s">
+      <c r="A6" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="55" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1855,7 +1855,7 @@
       <c r="J22" s="39"/>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>4</v>
       </c>
@@ -2700,11 +2700,11 @@
       <c r="B64" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C64" s="52">
+      <c r="C64" s="58">
         <f>J62</f>
         <v>252724.34732561468</v>
       </c>
-      <c r="D64" s="53"/>
+      <c r="D64" s="59"/>
       <c r="E64" s="15">
         <v>100</v>
       </c>
@@ -2719,21 +2719,21 @@
       <c r="B65" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="56">
+      <c r="C65" s="61">
         <v>225000</v>
       </c>
-      <c r="D65" s="57"/>
+      <c r="D65" s="62"/>
       <c r="E65" s="15"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="56">
+      <c r="C66" s="61">
         <f>C65-C68-C69</f>
         <v>213750</v>
       </c>
-      <c r="D66" s="57"/>
+      <c r="D66" s="62"/>
       <c r="E66" s="15">
         <f>C66/C64*100</f>
         <v>84.578317151453788</v>
@@ -2743,11 +2743,11 @@
       <c r="B67" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="58">
+      <c r="C67" s="63">
         <f>C64-C66</f>
         <v>38974.347325614683</v>
       </c>
-      <c r="D67" s="58"/>
+      <c r="D67" s="63"/>
       <c r="E67" s="15">
         <f>100-E66</f>
         <v>15.421682848546212</v>
@@ -2757,11 +2757,11 @@
       <c r="B68" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C68" s="52">
+      <c r="C68" s="58">
         <f>C65*0.03</f>
         <v>6750</v>
       </c>
-      <c r="D68" s="53"/>
+      <c r="D68" s="59"/>
       <c r="E68" s="15">
         <v>3</v>
       </c>
@@ -2770,24 +2770,17 @@
       <c r="B69" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="52">
+      <c r="C69" s="58">
         <f>C65*0.02</f>
         <v>4500</v>
       </c>
-      <c r="D69" s="53"/>
+      <c r="D69" s="59"/>
       <c r="E69" s="15">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="A7:F7"/>
@@ -2796,6 +2789,13 @@
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2833,90 +2833,90 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="F1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
+      <c r="B1" s="66"/>
+      <c r="C1" s="66"/>
+      <c r="D1" s="66"/>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="66"/>
+      <c r="I1" s="66"/>
+      <c r="J1" s="66"/>
+      <c r="K1" s="66"/>
     </row>
     <row r="2" spans="1:13" ht="25.5" x14ac:dyDescent="0.35">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="67" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="74"/>
-      <c r="C2" s="74"/>
-      <c r="D2" s="74"/>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
-      <c r="I2" s="74"/>
-      <c r="J2" s="74"/>
-      <c r="K2" s="74"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="67"/>
+      <c r="G2" s="67"/>
+      <c r="H2" s="67"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
     </row>
     <row r="3" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="75"/>
-      <c r="C5" s="75"/>
-      <c r="D5" s="75"/>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
-      <c r="I5" s="75"/>
-      <c r="J5" s="75"/>
-      <c r="K5" s="75"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="68"/>
+      <c r="D5" s="68"/>
+      <c r="E5" s="68"/>
+      <c r="F5" s="68"/>
+      <c r="G5" s="68"/>
+      <c r="H5" s="68"/>
+      <c r="I5" s="68"/>
+      <c r="J5" s="68"/>
+      <c r="K5" s="68"/>
     </row>
     <row r="6" spans="1:13" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>19</v>
       </c>
       <c r="B6" s="11"/>
-      <c r="C6" s="71">
+      <c r="C6" s="64">
         <f>F43</f>
         <v>254687.53618383879</v>
       </c>
-      <c r="D6" s="72"/>
+      <c r="D6" s="65"/>
       <c r="E6" s="12"/>
       <c r="F6" s="11"/>
       <c r="G6" s="11"/>
@@ -2924,11 +2924,11 @@
         <v>20</v>
       </c>
       <c r="I6" s="11"/>
-      <c r="J6" s="71">
+      <c r="J6" s="64">
         <f>I43</f>
         <v>244779.4861838388</v>
       </c>
-      <c r="K6" s="72"/>
+      <c r="K6" s="65"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="35" t="s">
@@ -2937,77 +2937,77 @@
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13"/>
-      <c r="F7" s="67"/>
-      <c r="G7" s="67"/>
-      <c r="I7" s="68" t="s">
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="I7" s="73" t="s">
         <v>46</v>
       </c>
-      <c r="J7" s="68"/>
-      <c r="K7" s="68"/>
+      <c r="J7" s="73"/>
+      <c r="K7" s="73"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="66" t="str">
+      <c r="A8" s="71" t="str">
         <f>new!A6</f>
         <v>Project:- Pasikhel pahiro roktham kaarya</v>
       </c>
-      <c r="B8" s="66"/>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66"/>
-      <c r="E8" s="66"/>
-      <c r="F8" s="66"/>
-      <c r="I8" s="69" t="s">
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="I8" s="74" t="s">
         <v>65</v>
       </c>
-      <c r="J8" s="69"/>
-      <c r="K8" s="69"/>
+      <c r="J8" s="74"/>
+      <c r="K8" s="74"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="66" t="str">
+      <c r="A9" s="71" t="str">
         <f>new!A7</f>
         <v>Location:- Shankharapur Municipality 9</v>
       </c>
-      <c r="B9" s="66"/>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66"/>
-      <c r="E9" s="66"/>
-      <c r="F9" s="66"/>
-      <c r="I9" s="69" t="s">
+      <c r="B9" s="71"/>
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="I9" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="J9" s="69"/>
-      <c r="K9" s="69"/>
+      <c r="J9" s="74"/>
+      <c r="K9" s="74"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B11" s="64" t="s">
+      <c r="B11" s="69" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="64" t="s">
+      <c r="C11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="70" t="s">
+      <c r="D11" s="75" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="70"/>
-      <c r="F11" s="70"/>
-      <c r="G11" s="70" t="s">
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="70"/>
-      <c r="I11" s="70"/>
-      <c r="J11" s="64" t="s">
+      <c r="H11" s="75"/>
+      <c r="I11" s="75"/>
+      <c r="J11" s="69" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="65" t="s">
+      <c r="K11" s="70" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="64"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
+      <c r="A12" s="69"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
       <c r="D12" s="14" t="s">
         <v>26</v>
       </c>
@@ -3026,8 +3026,8 @@
       <c r="I12" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="J12" s="64"/>
-      <c r="K12" s="65"/>
+      <c r="J12" s="69"/>
+      <c r="K12" s="70"/>
     </row>
     <row r="13" spans="1:13" s="1" customFormat="1" ht="120" x14ac:dyDescent="0.25">
       <c r="A13" s="36">
@@ -3911,13 +3911,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
     <mergeCell ref="J11:J12"/>
     <mergeCell ref="K11:K12"/>
     <mergeCell ref="A8:F8"/>
@@ -3931,6 +3924,13 @@
     <mergeCell ref="C11:C12"/>
     <mergeCell ref="D11:F11"/>
     <mergeCell ref="G11:I11"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3951,8 +3951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7:K7"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3971,114 +3971,114 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="str">
+      <c r="A6" s="52" t="str">
         <f>new!A6</f>
         <v>Project:- Pasikhel pahiro roktham kaarya</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
-      <c r="H6" s="55" t="s">
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
+      <c r="H6" s="53" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="55"/>
-      <c r="J6" s="55"/>
-      <c r="K6" s="55"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="2"/>
-      <c r="H7" s="55" t="s">
+      <c r="H7" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="I7" s="55"/>
-      <c r="J7" s="55"/>
-      <c r="K7" s="55"/>
+      <c r="I7" s="53"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="53"/>
     </row>
     <row r="8" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -4395,7 +4395,7 @@
       <c r="J22" s="39"/>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>4</v>
       </c>
@@ -5241,11 +5241,11 @@
       <c r="B64" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="52">
+      <c r="C64" s="58">
         <f>J62</f>
         <v>242816.29732561469</v>
       </c>
-      <c r="D64" s="53"/>
+      <c r="D64" s="59"/>
       <c r="E64" s="15">
         <v>100</v>
       </c>
@@ -5260,21 +5260,21 @@
       <c r="B65" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="56">
+      <c r="C65" s="61">
         <v>150000</v>
       </c>
-      <c r="D65" s="57"/>
+      <c r="D65" s="62"/>
       <c r="E65" s="15"/>
     </row>
     <row r="66" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B66" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="56">
+      <c r="C66" s="61">
         <f>84.58%*C64</f>
         <v>205374.02427800492</v>
       </c>
-      <c r="D66" s="57"/>
+      <c r="D66" s="62"/>
       <c r="E66" s="15">
         <f>C66/C64*100</f>
         <v>84.58</v>
@@ -5284,11 +5284,11 @@
       <c r="B67" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="58">
+      <c r="C67" s="63">
         <f>C64-C66</f>
         <v>37442.273047609779</v>
       </c>
-      <c r="D67" s="58"/>
+      <c r="D67" s="63"/>
       <c r="E67" s="15">
         <f>100-E66</f>
         <v>15.420000000000002</v>
@@ -5298,11 +5298,11 @@
       <c r="B68" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C68" s="52">
+      <c r="C68" s="58">
         <f>C65*0.03</f>
         <v>4500</v>
       </c>
-      <c r="D68" s="53"/>
+      <c r="D68" s="59"/>
       <c r="E68" s="15">
         <v>3</v>
       </c>
@@ -5311,17 +5311,24 @@
       <c r="B69" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="52">
+      <c r="C69" s="58">
         <f>C65*0.02</f>
         <v>3000</v>
       </c>
-      <c r="D69" s="53"/>
+      <c r="D69" s="59"/>
       <c r="E69" s="15">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="A7:F7"/>
@@ -5330,13 +5337,6 @@
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5354,7 +5354,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+    <sheetView topLeftCell="A47" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -5374,91 +5374,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="60"/>
-      <c r="C1" s="60"/>
-      <c r="D1" s="60"/>
-      <c r="E1" s="60"/>
-      <c r="F1" s="60"/>
-      <c r="G1" s="60"/>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="60"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
     </row>
     <row r="2" spans="1:11" s="1" customFormat="1" ht="22.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="61" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-      <c r="J2" s="61"/>
-      <c r="K2" s="61"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
     </row>
     <row r="3" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="62" t="s">
+      <c r="A3" s="56" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="62"/>
-      <c r="C3" s="62"/>
-      <c r="D3" s="62"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="62"/>
-      <c r="G3" s="62"/>
-      <c r="H3" s="62"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="62"/>
-      <c r="K3" s="62"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
+      <c r="G3" s="56"/>
+      <c r="H3" s="56"/>
+      <c r="I3" s="56"/>
+      <c r="J3" s="56"/>
+      <c r="K3" s="56"/>
     </row>
     <row r="4" spans="1:11" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="62" t="s">
+      <c r="A4" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="62"/>
-      <c r="C4" s="62"/>
-      <c r="D4" s="62"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="62"/>
-      <c r="G4" s="62"/>
-      <c r="H4" s="62"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="62"/>
-      <c r="K4" s="62"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
     </row>
     <row r="5" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="B5" s="63"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
+      <c r="B5" s="57"/>
+      <c r="C5" s="57"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
+      <c r="G5" s="57"/>
+      <c r="H5" s="57"/>
+      <c r="I5" s="57"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
     </row>
     <row r="6" spans="1:11" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="59" t="str">
+      <c r="A6" s="52" t="str">
         <f>new!A6</f>
         <v>Project:- Pasikhel pahiro roktham kaarya</v>
       </c>
-      <c r="B6" s="59"/>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="59"/>
-      <c r="F6" s="59"/>
-      <c r="G6" s="59"/>
+      <c r="B6" s="52"/>
+      <c r="C6" s="52"/>
+      <c r="D6" s="52"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="52"/>
+      <c r="G6" s="52"/>
       <c r="H6" s="76" t="s">
         <v>47</v>
       </c>
@@ -5467,14 +5467,14 @@
       <c r="K6" s="76"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="54" t="s">
+      <c r="A7" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="B7" s="54"/>
-      <c r="C7" s="54"/>
-      <c r="D7" s="54"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
+      <c r="B7" s="60"/>
+      <c r="C7" s="60"/>
+      <c r="D7" s="60"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="60"/>
       <c r="G7" s="2"/>
       <c r="H7" s="76" t="s">
         <v>48</v>
@@ -5798,7 +5798,7 @@
       <c r="J22" s="39"/>
       <c r="K22" s="31"/>
     </row>
-    <row r="23" spans="1:13" ht="120" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="105" x14ac:dyDescent="0.25">
       <c r="A23" s="28">
         <v>4</v>
       </c>
@@ -6644,11 +6644,11 @@
       <c r="B64" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="C64" s="52">
+      <c r="C64" s="58">
         <f>J62</f>
         <v>242816.29732561469</v>
       </c>
-      <c r="D64" s="53"/>
+      <c r="D64" s="59"/>
       <c r="E64" s="15">
         <v>100</v>
       </c>
@@ -6663,21 +6663,21 @@
       <c r="B65" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="C65" s="56">
+      <c r="C65" s="61">
         <v>150000</v>
       </c>
-      <c r="D65" s="57"/>
+      <c r="D65" s="62"/>
       <c r="E65" s="15"/>
     </row>
     <row r="66" spans="2:5" hidden="1" x14ac:dyDescent="0.25">
       <c r="B66" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="C66" s="56">
+      <c r="C66" s="61">
         <f>84.58%*C64</f>
         <v>205374.02427800492</v>
       </c>
-      <c r="D66" s="57"/>
+      <c r="D66" s="62"/>
       <c r="E66" s="15">
         <f>C66/C64*100</f>
         <v>84.58</v>
@@ -6687,11 +6687,11 @@
       <c r="B67" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C67" s="58">
+      <c r="C67" s="63">
         <f>C64-C66</f>
         <v>37442.273047609779</v>
       </c>
-      <c r="D67" s="58"/>
+      <c r="D67" s="63"/>
       <c r="E67" s="15">
         <f>100-E66</f>
         <v>15.420000000000002</v>
@@ -6701,11 +6701,11 @@
       <c r="B68" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="C68" s="52">
+      <c r="C68" s="58">
         <f>C65*0.03</f>
         <v>4500</v>
       </c>
-      <c r="D68" s="53"/>
+      <c r="D68" s="59"/>
       <c r="E68" s="15">
         <v>3</v>
       </c>
@@ -6714,17 +6714,24 @@
       <c r="B69" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="C69" s="52">
+      <c r="C69" s="58">
         <f>C65*0.02</f>
         <v>3000</v>
       </c>
-      <c r="D69" s="53"/>
+      <c r="D69" s="59"/>
       <c r="E69" s="15">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A2:K2"/>
+    <mergeCell ref="A3:K3"/>
+    <mergeCell ref="A4:K4"/>
+    <mergeCell ref="A5:K5"/>
     <mergeCell ref="C68:D68"/>
     <mergeCell ref="C69:D69"/>
     <mergeCell ref="A7:F7"/>
@@ -6733,13 +6740,6 @@
     <mergeCell ref="C65:D65"/>
     <mergeCell ref="C66:D66"/>
     <mergeCell ref="C67:D67"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A2:K2"/>
-    <mergeCell ref="A3:K3"/>
-    <mergeCell ref="A4:K4"/>
-    <mergeCell ref="A5:K5"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="H6:K6"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>